<commit_message>
Fixed the RX/TX lines between FTDI chip and ESP32 chip. 🤦‍♂
</commit_message>
<xml_diff>
--- a/femu/femu-1.0.1-parts01005.xlsx
+++ b/femu/femu-1.0.1-parts01005.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">PART</t>
   </si>
   <si>
-    <t xml:space="preserve">C12, C19, C22, C25, C27</t>
+    <t xml:space="preserve">C12,C19,C22,C25,C27</t>
   </si>
   <si>
     <t xml:space="preserve">GRM033C80J104KE84D</t>
@@ -142,7 +142,7 @@
     <t xml:space="preserve">C20</t>
   </si>
   <si>
-    <t xml:space="preserve">GRM022R60J103KE19L</t>
+    <t xml:space="preserve">01016D103KAT2A</t>
   </si>
   <si>
     <t xml:space="preserve">10pF</t>
@@ -172,10 +172,10 @@
     <t xml:space="preserve">1uF</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C2, C3, C15, C18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL03A105KQ3CSNH</t>
+    <t xml:space="preserve">C1,C2,C3,C15,C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMK063ABJ105KP-F</t>
   </si>
   <si>
     <t xml:space="preserve">2.4pF</t>
@@ -349,7 +349,7 @@
     <t xml:space="preserve">OSRAM RGB LED</t>
   </si>
   <si>
-    <t xml:space="preserve">LRTB R48G</t>
+    <t xml:space="preserve">LRTBR48G-P9Q7-1+R7S5-26+NP-68</t>
   </si>
   <si>
     <t xml:space="preserve">NCP167AFCT330T2G</t>
@@ -397,6 +397,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -480,8 +481,8 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H18" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -490,10 +491,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="24.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="59.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.51"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>

</xml_diff>